<commit_message>
Juegos de Ensayo descritos y añadido el del filtro
</commit_message>
<xml_diff>
--- a/JuegoPruebas/JuegoEnsayoAppMultas.xlsx
+++ b/JuegoPruebas/JuegoEnsayoAppMultas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>Juego de Prueba para AppMultas</t>
   </si>
@@ -93,6 +93,36 @@
   </si>
   <si>
     <t>DAR DE BAJA MULTA GENERADO ANTERIORMENTE</t>
+  </si>
+  <si>
+    <t>Listado multas &gt; Seleccionar multa&gt; Click en el boton "Anular Multa"</t>
+  </si>
+  <si>
+    <t>Multa que introduce un importe decimal, comprueba si acepta decimales</t>
+  </si>
+  <si>
+    <t>Comprueba si crea la multa correctamente cuando todos sus campos estan bien.</t>
+  </si>
+  <si>
+    <t>La matricula no existe, y tras meter una matricula que exista no te dejará crearla, ya que el importe tiene que ser numerico y el concepto tiene que tener mínimo 10 letras.</t>
+  </si>
+  <si>
+    <t>El concepto supera el límite de caracteres 255.</t>
+  </si>
+  <si>
+    <t>SALTAR FILTRO PARA COMPROBAR LA SEGURIDAD</t>
+  </si>
+  <si>
+    <t>/privado/index.jsp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruta </t>
+  </si>
+  <si>
+    <t>Descripción del juego de ensayo</t>
+  </si>
+  <si>
+    <t>El agente intentara entrar a la url "/privado/index.jsp" sin estar logueado. En este caso el filtro le mandara al login, mostrandole un mensaje que le notificará que para entrar a esa zona privada debe loguearse previamente.</t>
   </si>
 </sst>
 </file>
@@ -116,7 +146,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,8 +159,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -218,60 +254,159 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -553,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:G39"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43:G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,381 +700,458 @@
     <col min="4" max="4" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="31"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="7" t="s">
+      <c r="C5" s="29"/>
+      <c r="D5" s="37" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="14">
         <v>4321</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="5">
+      <c r="C6" s="14"/>
+      <c r="D6" s="4">
         <v>12345678</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="7" t="s">
+      <c r="C9" s="33"/>
+      <c r="D9" s="36" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="14">
         <v>1111</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="5">
+      <c r="C10" s="14"/>
+      <c r="D10" s="4">
         <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="13" t="s">
+      <c r="C13" s="33"/>
+      <c r="D13" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="11"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="35"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="10" t="s">
+      <c r="A14" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="18" t="s">
+      <c r="C14" s="7"/>
+      <c r="D14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="15"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="15"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="15"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="9"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="17"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="10" t="s">
+      <c r="A17" s="23"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="11"/>
+    </row>
+    <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="18">
+      <c r="C18" s="7"/>
+      <c r="D18" s="5">
         <v>49.99</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F18" s="14"/>
-      <c r="G18" s="15"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="9"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="15"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="9"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="15"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="9"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="17"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="11"/>
     </row>
     <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="13" t="s">
+      <c r="C24" s="29"/>
+      <c r="D24" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="11"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="10" t="s">
+      <c r="F24" s="29"/>
+      <c r="G24" s="31"/>
+    </row>
+    <row r="25" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="18">
+      <c r="C25" s="7"/>
+      <c r="D25" s="5">
         <v>150</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="15"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="9"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="15"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="9"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="15"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="9"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="17"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="10" t="s">
+      <c r="A28" s="18"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="11"/>
+    </row>
+    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="18">
+      <c r="C29" s="7"/>
+      <c r="D29" s="5">
         <v>49.99</v>
       </c>
-      <c r="E29" s="14" t="s">
+      <c r="E29" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="15"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="9"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="15"/>
+      <c r="A30" s="20"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="9"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="15"/>
+      <c r="A31" s="20"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="9"/>
     </row>
     <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="3"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="17"/>
+      <c r="A32" s="21"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="11"/>
     </row>
     <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="9"/>
-      <c r="D35" s="13" t="s">
+      <c r="C35" s="29"/>
+      <c r="D35" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E35" s="9" t="s">
+      <c r="E35" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="F35" s="9"/>
-      <c r="G35" s="11"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="31"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="10" t="s">
+      <c r="A36" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C36" s="10"/>
-      <c r="D36" s="18">
+      <c r="C36" s="7"/>
+      <c r="D36" s="5">
         <v>150</v>
       </c>
-      <c r="E36" s="14" t="s">
+      <c r="E36" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F36" s="14"/>
-      <c r="G36" s="15"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="9"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="15"/>
+      <c r="A37" s="17"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="9"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="15"/>
+      <c r="A38" s="17"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="9"/>
     </row>
     <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="3"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="17"/>
+      <c r="A39" s="18"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="11"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="16"/>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="25"/>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="27"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B43" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" s="42"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="43"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="40"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="9"/>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="41"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="E18:G21"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="E35:G35"/>
+  <mergeCells count="34">
+    <mergeCell ref="A41:G41"/>
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="B43:G45"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="E25:G28"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="E14:G17"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A18:A21"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="E36:G39"/>
     <mergeCell ref="B29:C29"/>
@@ -954,13 +1166,12 @@
     <mergeCell ref="E13:G13"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="E25:G28"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="E14:G17"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="E18:G21"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="E35:G35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>